<commit_message>
modify module register order and fix config's bug
Former-commit-id: 273f4d6c2a15c6dee2746bbd87d88a71f54656b4 [formerly 88988d719d0e52572525525eca6c94e291cafce2] [formerly d216a142c34c9d15b39a5b9ca47685815062bdad [formerly 4fa1bd9c9ac6929b43ffc5c1b47ffa0de05d42d5]]
Former-commit-id: c0fad3eadf13070667f1652469e5700a49bb9aba [formerly 5c0199d402e2e08ff6ab12b548ce81313355f388]
Former-commit-id: 13277dc6a3d0affd4149d41f4145283a60779612
</commit_message>
<xml_diff>
--- a/Bin/resource/excel/IObject.xlsx
+++ b/Bin/resource/excel/IObject.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20325"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\cpp\ArkGameFrame\Bin\Server\DataConfig\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\E\NF\ARK\Bin\resource\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{08E15241-30A4-42C1-98DF-54E7CC87C920}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="27525" windowHeight="17535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="468" windowWidth="27528" windowHeight="17532" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataNode" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525" concurrentCalc="0"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,12 +28,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
   <si>
     <t>Id</t>
-  </si>
-  <si>
-    <t>ID</t>
   </si>
   <si>
     <t>ClassName</t>
@@ -93,6 +91,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
     </font>
     <font>
@@ -100,11 +99,13 @@
       <sz val="11"/>
       <color indexed="8"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="9"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
     </font>
   </fonts>
@@ -651,79 +652,79 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A9" sqref="A9:N35"/>
+      <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="10.5" customWidth="1"/>
-    <col min="3" max="4" width="8.5" customWidth="1"/>
-    <col min="5" max="5" width="9.5" customWidth="1"/>
+    <col min="1" max="2" width="10.44140625" customWidth="1"/>
+    <col min="3" max="4" width="8.44140625" customWidth="1"/>
+    <col min="5" max="5" width="9.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="7" t="s">
+    </row>
+    <row r="2" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
         <v>5</v>
       </c>
+      <c r="B2" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="10" t="s">
+    <row r="3" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="10" t="s">
-        <v>7</v>
+      <c r="B3" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="C3" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="D3" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="E3" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="F3" s="10" t="b">
+        <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="8" t="s">
+    <row r="4" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
         <v>9</v>
-      </c>
-      <c r="B3" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="C3" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="D3" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="E3" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="F3" s="10" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="8" t="s">
-        <v>10</v>
       </c>
       <c r="B4" s="9" t="b">
         <v>1</v>
@@ -741,75 +742,75 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="C5" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="D5" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="E5" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="F5" s="10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="C5" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="D5" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="E5" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="F5" s="10" t="b">
+      <c r="B6" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="C6" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="D6" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="E6" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="F6" s="10" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="8" t="s">
+    <row r="7" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="C6" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="D6" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="E6" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="F6" s="10" t="b">
+      <c r="B7" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C7" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="D7" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="E7" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F7" s="3" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="11" t="s">
+    <row r="8" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
         <v>13</v>
-      </c>
-      <c r="B7" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="C7" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="D7" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="E7" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="F7" s="3" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="12" t="s">
-        <v>14</v>
       </c>
       <c r="B8" s="13"/>
       <c r="C8" s="13"/>
       <c r="D8" s="13"/>
       <c r="E8" s="13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F8" s="13"/>
     </row>

</xml_diff>

<commit_message>
replace the scene and group by map and instance; restructure KernelModule and MapModule
</commit_message>
<xml_diff>
--- a/Bin/resource/excel/IObject.xlsx
+++ b/Bin/resource/excel/IObject.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20325"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\E\NF\ARK\Bin\resource\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\opensource\ARK.net_header\Bin\resource\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{08E15241-30A4-42C1-98DF-54E7CC87C920}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="468" windowWidth="27528" windowHeight="17532" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="27525" windowHeight="17535"/>
   </bookViews>
   <sheets>
     <sheet name="DataNode" sheetId="1" r:id="rId1"/>
@@ -18,7 +17,7 @@
   <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
+      <x14:workbookPr defaultImageDpi="330"/>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
   <si>
     <t>Id</t>
   </si>
@@ -36,12 +35,6 @@
     <t>ClassName</t>
   </si>
   <si>
-    <t>SceneID</t>
-  </si>
-  <si>
-    <t>GroupID</t>
-  </si>
-  <si>
     <t>ConfigID</t>
   </si>
   <si>
@@ -72,13 +65,18 @@
     <t>Desc</t>
   </si>
   <si>
-    <t>0全局广播</t>
+    <t>MapID</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>InstanceID</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -647,22 +645,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
+      <selection pane="bottomLeft" activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="2" width="10.44140625" customWidth="1"/>
-    <col min="3" max="4" width="8.44140625" customWidth="1"/>
-    <col min="5" max="5" width="9.44140625" customWidth="1"/>
+    <col min="1" max="2" width="10.5" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -673,58 +673,58 @@
         <v>1</v>
       </c>
       <c r="D1" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="6" t="s">
+    </row>
+    <row r="2" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="B2" s="9" t="s">
         <v>4</v>
       </c>
+      <c r="C2" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="9" t="s">
+    <row r="3" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="10" t="s">
+      <c r="B3" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="C3" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="D3" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="E3" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="F3" s="10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="8" t="s">
         <v>7</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="10" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="C3" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="D3" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="E3" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="F3" s="10" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
-        <v>9</v>
       </c>
       <c r="B4" s="9" t="b">
         <v>1</v>
@@ -742,83 +742,81 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A5" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="C5" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="D5" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="E5" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="F5" s="10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="C6" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="D6" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="E6" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="F6" s="10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="C5" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="D5" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="E5" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="F5" s="10" t="b">
+      <c r="B7" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C7" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="D7" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="E7" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F7" s="3" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+    <row r="8" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="12" t="s">
         <v>11</v>
-      </c>
-      <c r="B6" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="C6" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="D6" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="E6" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="F6" s="10" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="C7" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="D7" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="E7" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="F7" s="3" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
-        <v>13</v>
       </c>
       <c r="B8" s="13"/>
       <c r="C8" s="13"/>
       <c r="D8" s="13"/>
-      <c r="E8" s="13" t="s">
-        <v>14</v>
-      </c>
+      <c r="E8" s="13"/>
       <c r="F8" s="13"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <dataValidations count="2">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1 A7" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7:J7 F2:F6 F8:F1048576" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1 A7"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7:J7 F2:F6 F8:F1048576">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>